<commit_message>
draw char for each employee's income
</commit_message>
<xml_diff>
--- a/info_employee.xlsx
+++ b/info_employee.xlsx
@@ -127,6 +127,1433 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$F$2:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="9" name="Chart 9"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="10" name="Chart 10"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId10"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="11" name="Chart 11"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="12" name="Chart 12"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="13" name="Chart 13"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId13"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="14" name="Chart 14"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="15" name="Chart 15"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="16" name="Chart 16"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId16"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="17" name="Chart 17"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId17"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>10</col>
+      <colOff>0</colOff>
+      <row>3</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="18" name="Chart 18"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId18"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,7 +1842,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -616,5 +2043,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>